<commit_message>
google - what, how, where working
</commit_message>
<xml_diff>
--- a/version1.0/Docs/Book1.xlsx
+++ b/version1.0/Docs/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zmlhq-my.sharepoint.com/personal/daisy_brown_zenmakerlab_com/Documents/Zen/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zmlhq-my.sharepoint.com/personal/daisy_brown_zenmakerlab_com/Documents/gitcobot/version1.0/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="13_ncr:1_{E0BB2951-155A-4C0E-9BA6-E84C03337BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F22B1E25-2C79-47E0-90E3-17F5E2AB6574}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="13_ncr:1_{E0BB2951-155A-4C0E-9BA6-E84C03337BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C2101D7-4F2C-4E97-B022-B184FAA95D8D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AE63D8C1-466B-4C26-A812-EDCDBB124742}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="195">
   <si>
     <t>Monday</t>
   </si>
@@ -575,6 +575,51 @@
   </si>
   <si>
     <t>reprinting bearing mounts in PETG 40%, including centre</t>
+  </si>
+  <si>
+    <t>working on drive mecgh</t>
+  </si>
+  <si>
+    <t>problems with cell 3</t>
+  </si>
+  <si>
+    <t>tested drive mech</t>
+  </si>
+  <si>
+    <t>bearing adapters are not holding</t>
+  </si>
+  <si>
+    <t>try install without shaft with set screws. Also add set screws from pla to shaft to stop horizontal motion</t>
+  </si>
+  <si>
+    <t>put drive mech together</t>
+  </si>
+  <si>
+    <t>working on battery</t>
+  </si>
+  <si>
+    <t>researching batteries</t>
+  </si>
+  <si>
+    <t>going with 2 4s 3300ma and 50C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">designing new battery mounts </t>
+  </si>
+  <si>
+    <t>created BOM</t>
+  </si>
+  <si>
+    <t>designed dome mounts</t>
+  </si>
+  <si>
+    <t>working with battery</t>
+  </si>
+  <si>
+    <t>found appropiate batteries</t>
+  </si>
+  <si>
+    <t>worked on wed scraping for clover to answer random questions</t>
   </si>
 </sst>
 </file>
@@ -976,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435AFAA3-9100-481B-8119-9D383E076530}">
-  <dimension ref="A1:N72"/>
+  <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,6 +1776,9 @@
       <c r="D69" s="3" t="s">
         <v>178</v>
       </c>
+      <c r="E69" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
@@ -1754,6 +1802,76 @@
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B77" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B78" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B79" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding webscraper to chatbot
</commit_message>
<xml_diff>
--- a/version1.0/Docs/Book1.xlsx
+++ b/version1.0/Docs/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zmlhq-my.sharepoint.com/personal/daisy_brown_zenmakerlab_com/Documents/gitcobot/version1.0/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="272" documentId="13_ncr:1_{E0BB2951-155A-4C0E-9BA6-E84C03337BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AE35B61-550B-4B6A-8E19-1EBE6A1A2CF2}"/>
+  <xr:revisionPtr revIDLastSave="278" documentId="13_ncr:1_{E0BB2951-155A-4C0E-9BA6-E84C03337BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CAF8B24-8C36-44B0-AF7C-60491E789C7F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AE63D8C1-466B-4C26-A812-EDCDBB124742}"/>
+    <workbookView minimized="1" xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{AE63D8C1-466B-4C26-A812-EDCDBB124742}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="232">
   <si>
     <t>Monday</t>
   </si>
@@ -716,6 +716,21 @@
   </si>
   <si>
     <t>put clover together with new batteries</t>
+  </si>
+  <si>
+    <t>fixed steering</t>
+  </si>
+  <si>
+    <t>tested new batteries and trailer</t>
+  </si>
+  <si>
+    <t>trailer is the weak point</t>
+  </si>
+  <si>
+    <t>integrated googling into chatbot</t>
+  </si>
+  <si>
+    <t>integrate google script</t>
   </si>
 </sst>
 </file>
@@ -1131,8 +1146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435AFAA3-9100-481B-8119-9D383E076530}">
   <dimension ref="A1:N109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,13 +2125,19 @@
       <c r="B104" s="3" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C104" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>215</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>221</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2126,16 +2147,25 @@
       <c r="B106" s="3" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C106" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>217</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>223</v>
       </c>
+      <c r="C107" s="3" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>231</v>
+      </c>
       <c r="B108" s="3" t="s">
         <v>224</v>
       </c>

</xml_diff>

<commit_message>
improving speechdata file format
</commit_message>
<xml_diff>
--- a/version1.0/Docs/Book1.xlsx
+++ b/version1.0/Docs/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zmlhq-my.sharepoint.com/personal/daisy_brown_zenmakerlab_com/Documents/gitcobot/version1.0/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="325" documentId="13_ncr:1_{E0BB2951-155A-4C0E-9BA6-E84C03337BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81D15C2A-48E0-41E4-88A6-B243701A127B}"/>
+  <xr:revisionPtr revIDLastSave="329" documentId="13_ncr:1_{E0BB2951-155A-4C0E-9BA6-E84C03337BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A74D978C-92CA-4AFE-9734-4C73AD3872E1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AE63D8C1-466B-4C26-A812-EDCDBB124742}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="263">
   <si>
     <t>Monday</t>
   </si>
@@ -812,6 +812,18 @@
   </si>
   <si>
     <t>also including reversing, still counts as distance</t>
+  </si>
+  <si>
+    <t>testing out adafruit magic circle</t>
+  </si>
+  <si>
+    <t>lots of possibility</t>
+  </si>
+  <si>
+    <t>sign shop trip</t>
+  </si>
+  <si>
+    <t>investigating adafruit bluefruit</t>
   </si>
 </sst>
 </file>
@@ -949,7 +961,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1695450</xdr:colOff>
-      <xdr:row>129</xdr:row>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>139854</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -984,6 +996,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1286,7 +1302,7 @@
   <dimension ref="A1:N141"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2375,13 +2391,19 @@
       <c r="C115" s="3" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D115" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>244</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>256</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2405,9 +2427,17 @@
         <v>247</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>248</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C121" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="133" spans="2:2" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
increasing vel limit, reducing calibration delays
</commit_message>
<xml_diff>
--- a/version1.0/Docs/Book1.xlsx
+++ b/version1.0/Docs/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zmlhq-my.sharepoint.com/personal/daisy_brown_zenmakerlab_com/Documents/gitcobot/version1.0/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="329" documentId="13_ncr:1_{E0BB2951-155A-4C0E-9BA6-E84C03337BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A74D978C-92CA-4AFE-9734-4C73AD3872E1}"/>
+  <xr:revisionPtr revIDLastSave="339" documentId="13_ncr:1_{E0BB2951-155A-4C0E-9BA6-E84C03337BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F61CC40-FCF5-4EEB-8BFD-DA38DCD0785B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AE63D8C1-466B-4C26-A812-EDCDBB124742}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="271">
   <si>
     <t>Monday</t>
   </si>
@@ -824,6 +824,30 @@
   </si>
   <si>
     <t>investigating adafruit bluefruit</t>
+  </si>
+  <si>
+    <t>fixing speech data file format</t>
+  </si>
+  <si>
+    <t>went to talmatora</t>
+  </si>
+  <si>
+    <t>kids loved the robot, notes:</t>
+  </si>
+  <si>
+    <t>webscraper didn’t provide any good answers, may be wise to remove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maybe use it for a separate game ? </t>
+  </si>
+  <si>
+    <t>some ideas:</t>
+  </si>
+  <si>
+    <t>Projector</t>
+  </si>
+  <si>
+    <t>lithim ions still stalling</t>
   </si>
 </sst>
 </file>
@@ -961,7 +985,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1695450</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>139854</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1302,7 +1326,7 @@
   <dimension ref="A1:N141"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+      <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2405,6 +2429,9 @@
       <c r="D116" s="3" t="s">
         <v>262</v>
       </c>
+      <c r="E116" s="3" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
@@ -2413,6 +2440,9 @@
       <c r="C117" s="3" t="s">
         <v>257</v>
       </c>
+      <c r="E117" s="3" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="118" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
@@ -2421,10 +2451,16 @@
       <c r="C118" s="3" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E118" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
         <v>247</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2434,10 +2470,31 @@
       <c r="C120" s="3" t="s">
         <v>259</v>
       </c>
+      <c r="E120" s="3" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C121" s="3" t="s">
         <v>260</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E122" s="3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E123" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E124" s="3" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="133" spans="2:2" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changing from listen to record
</commit_message>
<xml_diff>
--- a/version1.0/Docs/Book1.xlsx
+++ b/version1.0/Docs/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zmlhq-my.sharepoint.com/personal/daisy_brown_zenmakerlab_com/Documents/gitcobot/version1.0/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="339" documentId="13_ncr:1_{E0BB2951-155A-4C0E-9BA6-E84C03337BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F61CC40-FCF5-4EEB-8BFD-DA38DCD0785B}"/>
+  <xr:revisionPtr revIDLastSave="345" documentId="13_ncr:1_{E0BB2951-155A-4C0E-9BA6-E84C03337BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC6F22A7-6464-4C66-98FE-49886881B49F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AE63D8C1-466B-4C26-A812-EDCDBB124742}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="273">
   <si>
     <t>Monday</t>
   </si>
@@ -848,6 +848,12 @@
   </si>
   <si>
     <t>lithim ions still stalling</t>
+  </si>
+  <si>
+    <t>working on calibration, changing max vel</t>
+  </si>
+  <si>
+    <t>07/11/2022</t>
   </si>
 </sst>
 </file>
@@ -1323,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435AFAA3-9100-481B-8119-9D383E076530}">
-  <dimension ref="A1:N141"/>
+  <dimension ref="A1:N139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E125" sqref="E125"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2432,6 +2438,9 @@
       <c r="E116" s="3" t="s">
         <v>263</v>
       </c>
+      <c r="F116" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
@@ -2497,34 +2506,54 @@
         <v>270</v>
       </c>
     </row>
-    <row r="133" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B129" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B132" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B134" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="137" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="140" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B140" s="3" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="141" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B141" s="3" t="s">
         <v>254</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on adding buttons for jr robotics controls
</commit_message>
<xml_diff>
--- a/version1.0/Docs/Book1.xlsx
+++ b/version1.0/Docs/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zmlhq-my.sharepoint.com/personal/daisy_brown_zenmakerlab_com/Documents/gitcobot/version1.0/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="368" documentId="13_ncr:1_{E0BB2951-155A-4C0E-9BA6-E84C03337BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72F63C93-B736-4109-BD53-2C81645789A0}"/>
+  <xr:revisionPtr revIDLastSave="372" documentId="13_ncr:1_{E0BB2951-155A-4C0E-9BA6-E84C03337BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E5345EB-F954-4A94-B136-97AB5C03ABB3}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11175" xr2:uid="{AE63D8C1-466B-4C26-A812-EDCDBB124742}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AE63D8C1-466B-4C26-A812-EDCDBB124742}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="297">
   <si>
     <t>Monday</t>
   </si>
@@ -914,6 +914,18 @@
   </si>
   <si>
     <t>rebuilding top chassis</t>
+  </si>
+  <si>
+    <t>working on sending texts</t>
+  </si>
+  <si>
+    <t>pi sending messages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">working on envirnoment variables </t>
+  </si>
+  <si>
+    <t>set envirnoment variables</t>
   </si>
 </sst>
 </file>
@@ -1389,10 +1401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435AFAA3-9100-481B-8119-9D383E076530}">
-  <dimension ref="A1:N152"/>
+  <dimension ref="A1:N155"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B153" sqref="B153"/>
+      <selection activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2710,10 +2722,28 @@
       <c r="B151" s="3" t="s">
         <v>291</v>
       </c>
+      <c r="C151" s="3" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B152" s="3" t="s">
         <v>292</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B153" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B154" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B155" s="3" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>